<commit_message>
add timestamp to error log
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X907"/>
+  <dimension ref="A1:X908"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -83654,7 +83654,7 @@
       </c>
       <c r="C907" t="inlineStr">
         <is>
-          <t>227.61000000</t>
+          <t>227.75000000</t>
         </is>
       </c>
       <c r="D907" t="inlineStr">
@@ -83664,12 +83664,12 @@
       </c>
       <c r="E907" t="inlineStr">
         <is>
-          <t>226.30000000</t>
+          <t>223.05000000</t>
         </is>
       </c>
       <c r="F907" t="inlineStr">
         <is>
-          <t>359440.97052000</t>
+          <t>548551.87465000</t>
         </is>
       </c>
       <c r="G907" t="n">
@@ -83677,20 +83677,20 @@
       </c>
       <c r="H907" t="inlineStr">
         <is>
-          <t>79543484.38694170</t>
+          <t>122069507.65511160</t>
         </is>
       </c>
       <c r="I907" t="n">
-        <v>154783</v>
+        <v>257281</v>
       </c>
       <c r="J907" t="inlineStr">
         <is>
-          <t>185253.82840000</t>
+          <t>277426.26209000</t>
         </is>
       </c>
       <c r="K907" t="inlineStr">
         <is>
-          <t>41013852.01520870</t>
+          <t>61749990.22004080</t>
         </is>
       </c>
       <c r="L907" t="inlineStr">
@@ -83699,40 +83699,132 @@
         </is>
       </c>
       <c r="M907" t="n">
-        <v>226.2999999999994</v>
+        <v>223.0499999999994</v>
       </c>
       <c r="N907" t="n">
-        <v>224.8150000000002</v>
+        <v>223.1900000000002</v>
       </c>
       <c r="O907" t="n">
-        <v>204.8057142857131</v>
+        <v>204.3414285714274</v>
       </c>
       <c r="P907" t="n">
-        <v>188.6380000000004</v>
+        <v>188.4213333333337</v>
       </c>
       <c r="Q907" t="n">
-        <v>174.7906666666669</v>
+        <v>174.6823333333336</v>
       </c>
       <c r="R907" t="n">
-        <v>226.3</v>
+        <v>223.05</v>
       </c>
       <c r="S907" t="n">
-        <v>223.6500170906119</v>
+        <v>221.4833504239452</v>
       </c>
       <c r="T907" t="n">
-        <v>198.3418773958041</v>
+        <v>197.8418773958041</v>
       </c>
       <c r="U907" t="n">
-        <v>182.129643375708</v>
+        <v>181.8889026349672</v>
       </c>
       <c r="V907" t="n">
-        <v>16.21223402009616</v>
+        <v>15.95297476083692</v>
       </c>
       <c r="W907" t="n">
-        <v>11.97922534355007</v>
+        <v>11.92737349169822</v>
       </c>
       <c r="X907" t="n">
-        <v>4.233008676546094</v>
+        <v>4.025601269138702</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="1" t="n">
+        <v>906</v>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>223.01000000</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>230.65000000</t>
+        </is>
+      </c>
+      <c r="D908" t="inlineStr">
+        <is>
+          <t>222.86000000</t>
+        </is>
+      </c>
+      <c r="E908" t="inlineStr">
+        <is>
+          <t>226.01000000</t>
+        </is>
+      </c>
+      <c r="F908" t="inlineStr">
+        <is>
+          <t>236841.33489000</t>
+        </is>
+      </c>
+      <c r="G908" t="n">
+        <v>1581292799999</v>
+      </c>
+      <c r="H908" t="inlineStr">
+        <is>
+          <t>53961682.74622080</t>
+        </is>
+      </c>
+      <c r="I908" t="n">
+        <v>121551</v>
+      </c>
+      <c r="J908" t="inlineStr">
+        <is>
+          <t>118600.00134000</t>
+        </is>
+      </c>
+      <c r="K908" t="inlineStr">
+        <is>
+          <t>27024399.68038880</t>
+        </is>
+      </c>
+      <c r="L908" t="inlineStr">
+        <is>
+          <t>2020-02-09 08:00:00</t>
+        </is>
+      </c>
+      <c r="M908" t="n">
+        <v>226.0099999999994</v>
+      </c>
+      <c r="N908" t="n">
+        <v>224.5300000000001</v>
+      </c>
+      <c r="O908" t="n">
+        <v>209.7085714285702</v>
+      </c>
+      <c r="P908" t="n">
+        <v>192.798666666667</v>
+      </c>
+      <c r="Q908" t="n">
+        <v>177.3880000000002</v>
+      </c>
+      <c r="R908" t="n">
+        <v>226.01</v>
+      </c>
+      <c r="S908" t="n">
+        <v>224.5011168079817</v>
+      </c>
+      <c r="T908" t="n">
+        <v>202.1754347195266</v>
+      </c>
+      <c r="U908" t="n">
+        <v>185.1571320694141</v>
+      </c>
+      <c r="V908" t="n">
+        <v>17.0183026501125</v>
+      </c>
+      <c r="W908" t="n">
+        <v>12.94555932338108</v>
+      </c>
+      <c r="X908" t="n">
+        <v>4.072743326731421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the four hour MACD signal
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X918"/>
+  <dimension ref="A1:X921"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -84666,22 +84666,22 @@
       </c>
       <c r="C918" t="inlineStr">
         <is>
-          <t>282.94000000</t>
+          <t>285.00000000</t>
         </is>
       </c>
       <c r="D918" t="inlineStr">
         <is>
-          <t>274.20000000</t>
+          <t>251.56000000</t>
         </is>
       </c>
       <c r="E918" t="inlineStr">
         <is>
-          <t>281.50000000</t>
+          <t>258.45000000</t>
         </is>
       </c>
       <c r="F918" t="inlineStr">
         <is>
-          <t>259325.65012000</t>
+          <t>705973.72988000</t>
         </is>
       </c>
       <c r="G918" t="n">
@@ -84689,20 +84689,20 @@
       </c>
       <c r="H918" t="inlineStr">
         <is>
-          <t>72415979.83933530</t>
+          <t>191887955.75834830</t>
         </is>
       </c>
       <c r="I918" t="n">
-        <v>117736</v>
+        <v>298048</v>
       </c>
       <c r="J918" t="inlineStr">
         <is>
-          <t>129185.43359000</t>
+          <t>343303.10692000</t>
         </is>
       </c>
       <c r="K918" t="inlineStr">
         <is>
-          <t>36083461.40367740</t>
+          <t>93329064.50806450</t>
         </is>
       </c>
       <c r="L918" t="inlineStr">
@@ -84711,40 +84711,316 @@
         </is>
       </c>
       <c r="M918" t="n">
-        <v>281.4999999999993</v>
+        <v>258.4499999999992</v>
       </c>
       <c r="N918" t="n">
-        <v>282.0550000000001</v>
+        <v>270.5300000000001</v>
       </c>
       <c r="O918" t="n">
-        <v>272.7371428571417</v>
+        <v>269.4442857142846</v>
       </c>
       <c r="P918" t="n">
-        <v>248.4213333333337</v>
+        <v>246.8846666666671</v>
       </c>
       <c r="Q918" t="n">
-        <v>211.7400000000002</v>
+        <v>210.9716666666668</v>
       </c>
       <c r="R918" t="n">
-        <v>281.5</v>
+        <v>258.45</v>
       </c>
       <c r="S918" t="n">
-        <v>280.0251871234084</v>
+        <v>264.6585204567417</v>
       </c>
       <c r="T918" t="n">
-        <v>256.7962319932066</v>
+        <v>253.2500781470527</v>
       </c>
       <c r="U918" t="n">
-        <v>228.854682802849</v>
+        <v>227.1472753954416</v>
       </c>
       <c r="V918" t="n">
-        <v>27.94154919035753</v>
+        <v>26.10280275161111</v>
       </c>
       <c r="W918" t="n">
-        <v>24.86117750646197</v>
+        <v>24.49342821871268</v>
       </c>
       <c r="X918" t="n">
-        <v>3.080371683895567</v>
+        <v>1.609374532898425</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="1" t="n">
+        <v>917</v>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>258.44000000</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>264.33000000</t>
+        </is>
+      </c>
+      <c r="D919" t="inlineStr">
+        <is>
+          <t>245.34000000</t>
+        </is>
+      </c>
+      <c r="E919" t="inlineStr">
+        <is>
+          <t>256.96000000</t>
+        </is>
+      </c>
+      <c r="F919" t="inlineStr">
+        <is>
+          <t>972969.71691000</t>
+        </is>
+      </c>
+      <c r="G919" t="n">
+        <v>1582243199999</v>
+      </c>
+      <c r="H919" t="inlineStr">
+        <is>
+          <t>249383114.01101130</t>
+        </is>
+      </c>
+      <c r="I919" t="n">
+        <v>373551</v>
+      </c>
+      <c r="J919" t="inlineStr">
+        <is>
+          <t>494884.31858000</t>
+        </is>
+      </c>
+      <c r="K919" t="inlineStr">
+        <is>
+          <t>126895480.43393930</t>
+        </is>
+      </c>
+      <c r="L919" t="inlineStr">
+        <is>
+          <t>2020-02-20 08:00:00</t>
+        </is>
+      </c>
+      <c r="M919" t="n">
+        <v>256.9599999999992</v>
+      </c>
+      <c r="N919" t="n">
+        <v>257.7050000000001</v>
+      </c>
+      <c r="O919" t="n">
+        <v>267.8214285714274</v>
+      </c>
+      <c r="P919" t="n">
+        <v>250.4300000000004</v>
+      </c>
+      <c r="Q919" t="n">
+        <v>213.8873333333335</v>
+      </c>
+      <c r="R919" t="n">
+        <v>256.96</v>
+      </c>
+      <c r="S919" t="n">
+        <v>259.5261734855806</v>
+      </c>
+      <c r="T919" t="n">
+        <v>253.8208353551985</v>
+      </c>
+      <c r="U919" t="n">
+        <v>229.3556253661496</v>
+      </c>
+      <c r="V919" t="n">
+        <v>24.46520998904884</v>
+      </c>
+      <c r="W919" t="n">
+        <v>24.48778457277992</v>
+      </c>
+      <c r="X919" t="n">
+        <v>-0.02257458373107468</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="1" t="n">
+        <v>918</v>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>256.97000000</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>268.24000000</t>
+        </is>
+      </c>
+      <c r="D920" t="inlineStr">
+        <is>
+          <t>253.61000000</t>
+        </is>
+      </c>
+      <c r="E920" t="inlineStr">
+        <is>
+          <t>265.27000000</t>
+        </is>
+      </c>
+      <c r="F920" t="inlineStr">
+        <is>
+          <t>525827.87340000</t>
+        </is>
+      </c>
+      <c r="G920" t="n">
+        <v>1582329599999</v>
+      </c>
+      <c r="H920" t="inlineStr">
+        <is>
+          <t>137848242.42793050</t>
+        </is>
+      </c>
+      <c r="I920" t="n">
+        <v>214306</v>
+      </c>
+      <c r="J920" t="inlineStr">
+        <is>
+          <t>269791.13743000</t>
+        </is>
+      </c>
+      <c r="K920" t="inlineStr">
+        <is>
+          <t>70748990.19707250</t>
+        </is>
+      </c>
+      <c r="L920" t="inlineStr">
+        <is>
+          <t>2020-02-21 08:00:00</t>
+        </is>
+      </c>
+      <c r="M920" t="n">
+        <v>265.2699999999991</v>
+      </c>
+      <c r="N920" t="n">
+        <v>261.1150000000001</v>
+      </c>
+      <c r="O920" t="n">
+        <v>264.9814285714274</v>
+      </c>
+      <c r="P920" t="n">
+        <v>253.9020000000004</v>
+      </c>
+      <c r="Q920" t="n">
+        <v>217.1273333333335</v>
+      </c>
+      <c r="R920" t="n">
+        <v>265.27</v>
+      </c>
+      <c r="S920" t="n">
+        <v>263.3553911618602</v>
+      </c>
+      <c r="T920" t="n">
+        <v>255.5822453005526</v>
+      </c>
+      <c r="U920" t="n">
+        <v>232.0159494131015</v>
+      </c>
+      <c r="V920" t="n">
+        <v>23.56629588745108</v>
+      </c>
+      <c r="W920" t="n">
+        <v>24.30348683571415</v>
+      </c>
+      <c r="X920" t="n">
+        <v>-0.737190948263077</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="1" t="n">
+        <v>919</v>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>265.32000000</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>266.81000000</t>
+        </is>
+      </c>
+      <c r="D921" t="inlineStr">
+        <is>
+          <t>256.00000000</t>
+        </is>
+      </c>
+      <c r="E921" t="inlineStr">
+        <is>
+          <t>260.07000000</t>
+        </is>
+      </c>
+      <c r="F921" t="inlineStr">
+        <is>
+          <t>131198.45412000</t>
+        </is>
+      </c>
+      <c r="G921" t="n">
+        <v>1582415999999</v>
+      </c>
+      <c r="H921" t="inlineStr">
+        <is>
+          <t>34246889.54929590</t>
+        </is>
+      </c>
+      <c r="I921" t="n">
+        <v>56352</v>
+      </c>
+      <c r="J921" t="inlineStr">
+        <is>
+          <t>65789.53417000</t>
+        </is>
+      </c>
+      <c r="K921" t="inlineStr">
+        <is>
+          <t>17180024.14857720</t>
+        </is>
+      </c>
+      <c r="L921" t="inlineStr">
+        <is>
+          <t>2020-02-22 08:00:00</t>
+        </is>
+      </c>
+      <c r="M921" t="n">
+        <v>260.0699999999991</v>
+      </c>
+      <c r="N921" t="n">
+        <v>262.6700000000001</v>
+      </c>
+      <c r="O921" t="n">
+        <v>264.2942857142846</v>
+      </c>
+      <c r="P921" t="n">
+        <v>256.3513333333337</v>
+      </c>
+      <c r="Q921" t="n">
+        <v>220.3693333333335</v>
+      </c>
+      <c r="R921" t="n">
+        <v>260.07</v>
+      </c>
+      <c r="S921" t="n">
+        <v>261.1651303872868</v>
+      </c>
+      <c r="T921" t="n">
+        <v>256.2726691004675</v>
+      </c>
+      <c r="U921" t="n">
+        <v>234.0940272343533</v>
+      </c>
+      <c r="V921" t="n">
+        <v>22.17864186611425</v>
+      </c>
+      <c r="W921" t="n">
+        <v>23.87851784179417</v>
+      </c>
+      <c r="X921" t="n">
+        <v>-1.699875975679927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MACD Strategy mail Online
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X927"/>
+  <dimension ref="A1:X928"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -85504,12 +85504,12 @@
       </c>
       <c r="E927" t="inlineStr">
         <is>
-          <t>222.81000000</t>
+          <t>226.76000000</t>
         </is>
       </c>
       <c r="F927" t="inlineStr">
         <is>
-          <t>848128.28112000</t>
+          <t>1054994.92397000</t>
         </is>
       </c>
       <c r="G927" t="n">
@@ -85517,20 +85517,20 @@
       </c>
       <c r="H927" t="inlineStr">
         <is>
-          <t>189689733.37432200</t>
+          <t>236064804.33459430</t>
         </is>
       </c>
       <c r="I927" t="n">
-        <v>270666</v>
+        <v>347125</v>
       </c>
       <c r="J927" t="inlineStr">
         <is>
-          <t>407001.92892000</t>
+          <t>510185.33752000</t>
         </is>
       </c>
       <c r="K927" t="inlineStr">
         <is>
-          <t>91127855.04634910</t>
+          <t>114271376.01220230</t>
         </is>
       </c>
       <c r="L927" t="inlineStr">
@@ -85539,40 +85539,132 @@
         </is>
       </c>
       <c r="M927" t="n">
-        <v>222.8099999999991</v>
+        <v>226.7599999999991</v>
       </c>
       <c r="N927" t="n">
-        <v>225.3000000000001</v>
+        <v>227.2750000000001</v>
       </c>
       <c r="O927" t="n">
-        <v>246.1099999999988</v>
+        <v>246.6742857142846</v>
       </c>
       <c r="P927" t="n">
-        <v>257.5193333333337</v>
+        <v>257.7826666666671</v>
       </c>
       <c r="Q927" t="n">
-        <v>235.4530000000001</v>
+        <v>235.5846666666668</v>
       </c>
       <c r="R927" t="n">
-        <v>222.81</v>
+        <v>226.76</v>
       </c>
       <c r="S927" t="n">
-        <v>225.1360289854421</v>
+        <v>227.7693623187754</v>
       </c>
       <c r="T927" t="n">
-        <v>244.9882017112183</v>
+        <v>245.5958940189106</v>
       </c>
       <c r="U927" t="n">
-        <v>236.7368720545731</v>
+        <v>237.0294646471656</v>
       </c>
       <c r="V927" t="n">
-        <v>8.251329656645254</v>
+        <v>8.566429371744988</v>
       </c>
       <c r="W927" t="n">
-        <v>16.56183150763261</v>
+        <v>16.62485145065256</v>
       </c>
       <c r="X927" t="n">
-        <v>-8.310501850987357</v>
+        <v>-8.058422078907572</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="1" t="n">
+        <v>926</v>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>226.76000000</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>233.00000000</t>
+        </is>
+      </c>
+      <c r="D928" t="inlineStr">
+        <is>
+          <t>226.66000000</t>
+        </is>
+      </c>
+      <c r="E928" t="inlineStr">
+        <is>
+          <t>227.77000000</t>
+        </is>
+      </c>
+      <c r="F928" t="inlineStr">
+        <is>
+          <t>190005.45453000</t>
+        </is>
+      </c>
+      <c r="G928" t="n">
+        <v>1583020799999</v>
+      </c>
+      <c r="H928" t="inlineStr">
+        <is>
+          <t>43646913.58164920</t>
+        </is>
+      </c>
+      <c r="I928" t="n">
+        <v>72779</v>
+      </c>
+      <c r="J928" t="inlineStr">
+        <is>
+          <t>95828.97252000</t>
+        </is>
+      </c>
+      <c r="K928" t="inlineStr">
+        <is>
+          <t>22017960.69998580</t>
+        </is>
+      </c>
+      <c r="L928" t="inlineStr">
+        <is>
+          <t>2020-02-29 08:00:00</t>
+        </is>
+      </c>
+      <c r="M928" t="n">
+        <v>227.7699999999991</v>
+      </c>
+      <c r="N928" t="n">
+        <v>227.2650000000001</v>
+      </c>
+      <c r="O928" t="n">
+        <v>241.8457142857132</v>
+      </c>
+      <c r="P928" t="n">
+        <v>253.9573333333337</v>
+      </c>
+      <c r="Q928" t="n">
+        <v>237.0206666666668</v>
+      </c>
+      <c r="R928" t="n">
+        <v>227.77</v>
+      </c>
+      <c r="S928" t="n">
+        <v>227.7697874395918</v>
+      </c>
+      <c r="T928" t="n">
+        <v>242.8534487852321</v>
+      </c>
+      <c r="U928" t="n">
+        <v>236.3435783770052</v>
+      </c>
+      <c r="V928" t="n">
+        <v>6.509870408226845</v>
+      </c>
+      <c r="W928" t="n">
+        <v>14.60185524216742</v>
+      </c>
+      <c r="X928" t="n">
+        <v>-8.091984833940572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the Data retrieve time to reduce the execute time
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -86690,22 +86690,22 @@
       </c>
       <c r="C940" t="inlineStr">
         <is>
-          <t>195.35000000</t>
+          <t>195.55000000</t>
         </is>
       </c>
       <c r="D940" t="inlineStr">
         <is>
-          <t>194.59000000</t>
+          <t>123.00000000</t>
         </is>
       </c>
       <c r="E940" t="inlineStr">
         <is>
-          <t>195.24000000</t>
+          <t>140.25000000</t>
         </is>
       </c>
       <c r="F940" t="inlineStr">
         <is>
-          <t>5122.98523000</t>
+          <t>2360255.43959000</t>
         </is>
       </c>
       <c r="G940" t="n">
@@ -86713,20 +86713,20 @@
       </c>
       <c r="H940" t="inlineStr">
         <is>
-          <t>999459.47850310</t>
+          <t>361226535.60061320</t>
         </is>
       </c>
       <c r="I940" t="n">
-        <v>1226</v>
+        <v>565370</v>
       </c>
       <c r="J940" t="inlineStr">
         <is>
-          <t>2383.01743000</t>
+          <t>1120307.78494000</t>
         </is>
       </c>
       <c r="K940" t="inlineStr">
         <is>
-          <t>464786.72242250</t>
+          <t>171376434.58774650</t>
         </is>
       </c>
       <c r="L940" t="inlineStr">
@@ -86735,40 +86735,40 @@
         </is>
       </c>
       <c r="M940" t="n">
-        <v>195.2399999999991</v>
+        <v>140.2499999999991</v>
       </c>
       <c r="N940" t="n">
-        <v>194.9250000000002</v>
+        <v>167.4300000000002</v>
       </c>
       <c r="O940" t="n">
-        <v>210.6999999999989</v>
+        <v>202.8442857142846</v>
       </c>
       <c r="P940" t="n">
-        <v>218.1993333333337</v>
+        <v>214.5333333333337</v>
       </c>
       <c r="Q940" t="n">
-        <v>240.6413333333336</v>
+        <v>238.8083333333336</v>
       </c>
       <c r="R940" t="n">
-        <v>195.24</v>
+        <v>140.25</v>
       </c>
       <c r="S940" t="n">
-        <v>195.9010075432408</v>
+        <v>159.2410075432408</v>
       </c>
       <c r="T940" t="n">
-        <v>213.9487679337884</v>
+        <v>205.4887679337884</v>
       </c>
       <c r="U940" t="n">
-        <v>222.296367226898</v>
+        <v>218.2230338935646</v>
       </c>
       <c r="V940" t="n">
-        <v>-8.347599293109511</v>
+        <v>-12.73426595977617</v>
       </c>
       <c r="W940" t="n">
-        <v>-2.704268726399379</v>
+        <v>-3.581602059732711</v>
       </c>
       <c r="X940" t="n">
-        <v>-5.643330566710132</v>
+        <v>-9.152663900043455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20200317 Add the different situation email
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X44"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4263,17 +4263,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>125.18000000</t>
+          <t>120.00000000</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>128.05000000</t>
+          <t>122.54000000</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>934109.27023000</t>
+          <t>1237674.88642000</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -4281,20 +4281,20 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>121064923.49606690</t>
+          <t>159192895.55261970</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>301396</v>
+        <v>398146</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>477998.58445000</t>
+          <t>628481.86635000</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>61956083.79341620</t>
+          <t>80877487.98928390</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -4303,40 +4303,224 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>128.0499999999998</v>
+        <v>122.5399999999998</v>
       </c>
       <c r="N44" t="n">
-        <v>131.0550000000001</v>
+        <v>128.3000000000001</v>
       </c>
       <c r="O44" t="n">
-        <v>166.7828571428571</v>
+        <v>165.9957142857143</v>
       </c>
       <c r="P44" t="n">
-        <v>199.542</v>
+        <v>199.1746666666667</v>
       </c>
       <c r="Q44" t="n">
-        <v>228.6623333333334</v>
+        <v>228.4786666666668</v>
       </c>
       <c r="R44" t="n">
-        <v>128.05</v>
+        <v>122.54</v>
       </c>
       <c r="S44" t="n">
-        <v>130.4490008381379</v>
+        <v>126.7756675048045</v>
       </c>
       <c r="T44" t="n">
-        <v>180.7116821032397</v>
+        <v>179.8633457903535</v>
       </c>
       <c r="U44" t="n">
-        <v>205.2637722529085</v>
+        <v>204.8401443871479</v>
       </c>
       <c r="V44" t="n">
-        <v>-24.55209014966886</v>
+        <v>-24.97679859679442</v>
       </c>
       <c r="W44" t="n">
-        <v>-13.67199895507777</v>
+        <v>-13.75694642572816</v>
       </c>
       <c r="X44" t="n">
-        <v>-10.88009119459108</v>
+        <v>-11.21985217106626</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>122.54000000</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>133.50000000</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>120.16000000</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>123.78000000</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>1312950.90137000</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>1584316799999</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>163436235.26909020</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>346579</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>669525.68240000</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>83359166.35016240</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>2020-03-15 08:00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>123.7799999999998</v>
+      </c>
+      <c r="N45" t="n">
+        <v>123.1600000000001</v>
+      </c>
+      <c r="O45" t="n">
+        <v>155.1885714285714</v>
+      </c>
+      <c r="P45" t="n">
+        <v>192.946</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>223.0996666666668</v>
+      </c>
+      <c r="R45" t="n">
+        <v>123.78</v>
+      </c>
+      <c r="S45" t="n">
+        <v>124.7785558349348</v>
+      </c>
+      <c r="T45" t="n">
+        <v>171.229592868324</v>
+      </c>
+      <c r="U45" t="n">
+        <v>198.6254195632536</v>
+      </c>
+      <c r="V45" t="n">
+        <v>-27.39582669492958</v>
+      </c>
+      <c r="W45" t="n">
+        <v>-16.48487100190949</v>
+      </c>
+      <c r="X45" t="n">
+        <v>-10.91095569302009</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>123.82000000</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>124.33000000</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>101.10000000</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>111.18000000</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>1778230.76646000</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>1584403199999</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>196383322.33181800</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>466021</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>864592.43860000</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>95415716.67891000</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>2020-03-16 08:00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>111.1799999999998</v>
+      </c>
+      <c r="N46" t="n">
+        <v>117.48</v>
+      </c>
+      <c r="O46" t="n">
+        <v>142.0985714285714</v>
+      </c>
+      <c r="P46" t="n">
+        <v>185.8373333333333</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>217.9763333333334</v>
+      </c>
+      <c r="R46" t="n">
+        <v>111.18</v>
+      </c>
+      <c r="S46" t="n">
+        <v>115.7128519449783</v>
+      </c>
+      <c r="T46" t="n">
+        <v>161.9861699288043</v>
+      </c>
+      <c r="U46" t="n">
+        <v>191.9384938731846</v>
+      </c>
+      <c r="V46" t="n">
+        <v>-29.95232394438028</v>
+      </c>
+      <c r="W46" t="n">
+        <v>-19.17847891357495</v>
+      </c>
+      <c r="X46" t="n">
+        <v>-10.77384503080534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>